<commit_message>
Updating and Refactor Code
</commit_message>
<xml_diff>
--- a/storage/aging-rate-2022.xlsx
+++ b/storage/aging-rate-2022.xlsx
@@ -263,7 +263,7 @@
     <t>Berdasarkan pengalaman, LGD (kerugian) yang akan terjadi setelah AR masuk kategori kualitas "macet" adalah 100% karena tagihan tidak mempunyai jaminan (collateral)</t>
   </si>
   <si>
-    <t>STEP #1 isi angka kualitas AR dari bulan Januari 2021  -  Aug 2022</t>
+    <t>STEP #1 isi angka kualitas AR dari bulan Januari 2021  -  Sep 2022</t>
   </si>
 </sst>
 </file>
@@ -17195,7 +17195,7 @@
         <v>1668190000.0</v>
       </c>
       <c r="V4" s="6">
-        <v>0.0</v>
+        <v>1865514000.0</v>
       </c>
       <c r="W4" s="6">
         <v>0.0</v>
@@ -17275,7 +17275,7 @@
         <v>521867993.0</v>
       </c>
       <c r="V5" s="6">
-        <v>0.0</v>
+        <v>526249500.0</v>
       </c>
       <c r="W5" s="6">
         <v>0.0</v>
@@ -17355,7 +17355,7 @@
         <v>917819380.0</v>
       </c>
       <c r="V6" s="6">
-        <v>0.0</v>
+        <v>977393380.0</v>
       </c>
       <c r="W6" s="6">
         <v>0.0</v>
@@ -17435,7 +17435,7 @@
         <v>1234379140.0</v>
       </c>
       <c r="V7" s="6">
-        <v>0.0</v>
+        <v>1442604640.0</v>
       </c>
       <c r="W7" s="6">
         <v>0.0</v>
@@ -17451,71 +17451,73 @@
       </c>
     </row>
     <row r="8" spans="1:16155">
-      <c r="A8" s="9"/>
+      <c r="A8" s="9">
+        <v>0.0</v>
+      </c>
       <c r="B8" s="10"/>
       <c r="C8" s="11"/>
       <c r="D8" s="12">
+        <v>0.0</v>
+      </c>
+      <c r="E8" s="12">
         <v>21094500.0</v>
       </c>
-      <c r="E8" s="12">
+      <c r="F8" s="12">
         <v>32067480.0</v>
       </c>
-      <c r="F8" s="12">
+      <c r="G8" s="12">
         <v>-12559000.0</v>
       </c>
-      <c r="G8" s="12">
+      <c r="H8" s="12">
         <v>18040996.0</v>
       </c>
-      <c r="H8" s="12">
+      <c r="I8" s="12">
         <v>45577214.0</v>
       </c>
-      <c r="I8" s="12">
+      <c r="J8" s="12">
         <v>9105000.0</v>
       </c>
-      <c r="J8" s="12">
+      <c r="K8" s="12">
         <v>1353000.0</v>
       </c>
-      <c r="K8" s="12">
+      <c r="L8" s="12">
         <v>-2411000.0</v>
       </c>
-      <c r="L8" s="12">
+      <c r="M8" s="12">
         <v>635954988.0</v>
       </c>
-      <c r="M8" s="12">
+      <c r="N8" s="12">
         <v>168231959.0</v>
       </c>
-      <c r="N8" s="12">
+      <c r="O8" s="12">
         <v>-917340375.0</v>
       </c>
-      <c r="O8" s="12">
+      <c r="P8" s="12">
         <v>10844000.0</v>
       </c>
-      <c r="P8" s="12">
+      <c r="Q8" s="12">
         <v>-70878980.0</v>
       </c>
-      <c r="Q8" s="12">
+      <c r="R8" s="12">
         <v>44126000.0</v>
       </c>
-      <c r="R8" s="12">
+      <c r="S8" s="12">
         <v>54577000.0</v>
       </c>
-      <c r="S8" s="12">
+      <c r="T8" s="12">
         <v>40290000.0</v>
       </c>
-      <c r="T8" s="12">
+      <c r="U8" s="12">
         <v>36209880.0</v>
       </c>
-      <c r="U8" s="12">
+      <c r="V8" s="12">
         <v>-43491500.0</v>
       </c>
-      <c r="V8" s="12">
-        <v>-1234379140.0</v>
-      </c>
       <c r="W8" s="12">
-        <v>0.0</v>
+        <v>208225500.0</v>
       </c>
       <c r="X8" s="12">
-        <v>0.0</v>
+        <v>-1442604640.0</v>
       </c>
       <c r="Y8" s="12">
         <v>0.0</v>
@@ -17586,7 +17588,7 @@
         <v>4342256513.0</v>
       </c>
       <c r="V9" s="15">
-        <v>0.0</v>
+        <v>4811761520.0</v>
       </c>
       <c r="W9" s="15">
         <v>0.0</v>
@@ -17726,13 +17728,13 @@
         <v>28.6220033834</v>
       </c>
       <c r="U13" s="23">
-        <v>53.2270750818</v>
+        <v>28.7407305523</v>
       </c>
       <c r="V13" s="23">
-        <v>53.2270750818</v>
+        <v>0.0</v>
       </c>
       <c r="W13" s="23">
-        <v>99.9999999999</v>
+        <v>50.2508201614</v>
       </c>
       <c r="X13" s="23">
         <v>99.9999999999</v>
@@ -17741,7 +17743,7 @@
         <v>99.9999999999</v>
       </c>
       <c r="Z13" s="23">
-        <v>0.0</v>
+        <v>50.1288459753</v>
       </c>
     </row>
     <row r="14" spans="1:16155" customHeight="1" ht="30.75">
@@ -17791,7 +17793,7 @@
         <v>70.5260344225</v>
       </c>
       <c r="Q14" s="23">
-        <v>0.0</v>
+        <v>75.0769551684</v>
       </c>
       <c r="R14" s="23">
         <v>0.0</v>
@@ -17803,13 +17805,13 @@
         <v>0.0</v>
       </c>
       <c r="U14" s="23">
-        <v>30.5405326963</v>
+        <v>0.0</v>
       </c>
       <c r="V14" s="24">
-        <v>30.5405326963</v>
+        <v>0.0</v>
       </c>
       <c r="W14" s="24">
-        <v>0.0</v>
+        <v>34.4919513894</v>
       </c>
       <c r="X14" s="24">
         <v>0.0</v>
@@ -17818,7 +17820,7 @@
         <v>0.0</v>
       </c>
       <c r="Z14" s="23">
-        <v>0.0</v>
+        <v>34.4919513894</v>
       </c>
     </row>
     <row r="15" spans="1:16155" customHeight="1" ht="30.75">
@@ -17874,19 +17876,19 @@
         <v>0.0</v>
       </c>
       <c r="S15" s="23">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="T15" s="23">
         <v>0.0</v>
       </c>
       <c r="U15" s="23">
-        <v>10.9713501759</v>
+        <v>0.0</v>
       </c>
       <c r="V15" s="23">
-        <v>10.9713501759</v>
+        <v>0.0</v>
       </c>
       <c r="W15" s="23">
-        <v>0.0</v>
+        <v>11.0189692235</v>
       </c>
       <c r="X15" s="24">
         <v>0.0</v>
@@ -17895,7 +17897,7 @@
         <v>0.0</v>
       </c>
       <c r="Z15" s="23">
-        <v>0.0</v>
+        <v>11.0189692235</v>
       </c>
     </row>
     <row r="18" spans="1:16155" customHeight="1" ht="45">
@@ -17935,7 +17937,7 @@
       </c>
       <c r="C19" s="23"/>
       <c r="D19" s="29">
-        <v>1.78348428</v>
+        <v>1.90986157</v>
       </c>
       <c r="E19" s="23"/>
       <c r="F19" s="30"/>
@@ -17956,7 +17958,7 @@
       </c>
       <c r="C20" s="23"/>
       <c r="D20" s="23">
-        <v>3.3507087877</v>
+        <v>3.8006575082</v>
       </c>
       <c r="E20" s="23"/>
       <c r="F20" s="30"/>
@@ -17972,9 +17974,7 @@
         <v>32</v>
       </c>
       <c r="C21" s="23"/>
-      <c r="D21" s="23">
-        <v>10.9713501759</v>
-      </c>
+      <c r="D21" s="23"/>
       <c r="E21" s="23"/>
       <c r="F21" s="30"/>
       <c r="G21" s="31"/>

</xml_diff>